<commit_message>
sql data type playing
</commit_message>
<xml_diff>
--- a/sqllab/earthquakeData.xlsx
+++ b/sqllab/earthquakeData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://carletoncollegemn-my.sharepoint.com/personal/sonr_carleton_edu/Documents/GitHub/cs257/sqllab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{17E7CF78-EDC6-C94F-A1F4-84B12D0C7B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{CCD1B4BA-C160-C04E-912C-67CFE30E061A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="21380"/>
   </bookViews>
@@ -11161,8 +11161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1840"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1675" workbookViewId="0">
-      <selection activeCell="J1702" sqref="J1702"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>